<commit_message>
all the changes pushed
</commit_message>
<xml_diff>
--- a/Excel_data/POC2DATASHEET.xlsx
+++ b/Excel_data/POC2DATASHEET.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Test case id</t>
   </si>
@@ -43,45 +43,15 @@
     <t>TC001</t>
   </si>
   <si>
-    <t>select Customer_Segment as'Customer Segment',Product_Category as 'Product Category',
-ROUND(sum(unit_Price),2) "Sum of Unit Price" from Superstoretesting
-group by Customer_Segment, Product_Category
-order by Customer_Segment, Product_Category asc</t>
-  </si>
-  <si>
-    <t>Dashboard data of Powe BI dashoard Testing 1 and  Database Qurry 1 data are matching</t>
-  </si>
-  <si>
     <t>TC002</t>
   </si>
   <si>
-    <t>Dashboard data of Powe BI dashoard Testing 2 and  Database Qurry 2 data are matching</t>
-  </si>
-  <si>
     <t>TC003</t>
   </si>
   <si>
-    <t>Compare the Dashboard data of Powe BI dashoard Testing 3 Vs Database Query 3 data</t>
-  </si>
-  <si>
-    <t>select Customer_Segment as 'Customer Segment',
-Product_Category as 'Product Category', 
-ROUND(sum(unit_Price),2) as 'Sum of Unit Price' 
-from Superstoretesting
-where Product_Category = 'Furniture'
-group by Customer_Segment, Product_Category
-order by Customer_Segment asc</t>
-  </si>
-  <si>
-    <t>Dashboard data of Powe BI dashoard Testing 3 and  Database Qurry 3 data are matching</t>
-  </si>
-  <si>
     <t>TC004</t>
   </si>
   <si>
-    <t>Compare the Dashboard data of Powe BI dashoard Testing 4 Vs Database Query 4  data</t>
-  </si>
-  <si>
     <t>Dashboard data of Powe BI dashoard Testing 4 and  Database Qurry 4 data are matching</t>
   </si>
   <si>
@@ -92,9 +62,6 @@
   </si>
   <si>
     <t>maheshchothve1997@gmail.com</t>
-  </si>
-  <si>
-    <t>Compare the Dashboard data of Powe BI dashoard Testing COURSE NAME Vs Database Query 1 data COURSENAME</t>
   </si>
   <si>
     <t>SELECT TOP (1000) 
@@ -102,18 +69,89 @@
   FROM [POC2].[dbo].[dim_institute]</t>
   </si>
   <si>
-    <t>Compare theInstitute name Dashboard data of Powe BI dashoard Testing 2 Vs Database Query 2 data</t>
+    <t>Compare the Dashboard data of Powe BI dashoard Testing Institute NAME Vs Database Query 1 data COURSENAME</t>
+  </si>
+  <si>
+    <t>Dashboard data of Powe BI dashoard Testing 1 and  Database Query 1 data are matching</t>
+  </si>
+  <si>
+    <t>Compare the Course name Dashboard data of Powe BI dashoard Testing 2 Vs Database Query 2 data</t>
+  </si>
+  <si>
+    <t>Dashboard data of Powe BI dashoard Testing 2 and  Database Query 2 data are matching</t>
+  </si>
+  <si>
+    <t>Compare the semister name Dashboard data of Powe BI dashoard Testing 3 Vs Database Query3 data</t>
+  </si>
+  <si>
+    <t>Dashboard data of Powe BI dashoard Testing 3 and  Database Query 3 data are matching</t>
+  </si>
+  <si>
+    <t>Compare the Subject name if course name= Computer Engineering  
+Sem=1
+Dashboard data of Powe BI dashoard Testing 4 Vs Database Query4 data</t>
+  </si>
+  <si>
+    <t>SELECT TOP (1000) 
+      [Subject_name]
+  FROM [POC2].[dbo].[Dim_Subject]
+  where course=20 AND sem=1 order by [Subject_name] asc;</t>
+  </si>
+  <si>
+    <t>TC005</t>
+  </si>
+  <si>
+    <t>Compare the  LECTURER name  if course name= Computer Engineering  
+Sem=1 and subject= Computer Engineering Dashboard data of Powe BI dashoard Testing 5 Vs Database Query5  data</t>
+  </si>
+  <si>
+    <t>SELECT DISTINCT TOP (1000)
+      [Lecturer_name]
+    FROM [POC2].[dbo].[dim_lecturer],[POC2].[dbo].[Dim_Subject]
+ WHERE  course=20 AND sem=1 AND [Subject_id]=112 AND [Lecturer_id]=22020212</t>
+  </si>
+  <si>
+    <t>Dashboard data of Powe BI dashoard Testing 5 and  Database Qurry 5 data are matching</t>
+  </si>
+  <si>
+    <t>TC006</t>
+  </si>
+  <si>
+    <t>Compare the Student name  if course name= Computer Engineering  
+Sem=1 and subject= Computer Engineering And lecturer is V.V. Marathe  Dashboard data of Powe BI dashoard Testing 6 Vs Database Query 6  data</t>
+  </si>
+  <si>
+    <t>SELECT TOP (1000) [Student_name]
+       FROM [POC2].[dbo].[dim_student]
+INNER JOIN  [POC2].[dbo].[fact_exam_new] 
+ON [dim_student].[Enrollment_No]=[fact_exam_new].[Enrollment_No] WHERE
+[Course_id]=20 AND [Subject_id]=112 ORDER BY Student_name asc</t>
+  </si>
+  <si>
+    <t>Dashboard data of Powe BI dashoard Testing 6 and  Database Qurry 6 data are matching</t>
+  </si>
+  <si>
+    <t>TC007</t>
+  </si>
+  <si>
+    <t>Compare the Year Dashboard data of Powe BI dashoard Testing 7 Vs Database Query 7 data</t>
+  </si>
+  <si>
+    <t>SELECT DISTINCT YEAR([Start_date]) AS Year FROM [POC2].[dbo].[fact_learning]</t>
+  </si>
+  <si>
+    <t>Dashboard data of Powe BI dashoard Testing 7 and  Database Qurry 7 data are matching</t>
   </si>
   <si>
     <t>SELECT TOP (1000)     [Course_name]
-  FROM [POC2].[dbo].[dim_course]</t>
+  FROM [POC2].[dbo].[dim_course] order by Course_name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -143,6 +181,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -164,7 +208,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -244,17 +288,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -276,19 +309,6 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -350,7 +370,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -367,10 +387,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -380,54 +400,60 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -710,10 +736,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -722,7 +748,7 @@
     <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="36.140625" style="10" customWidth="1"/>
     <col min="4" max="4" width="33.85546875" customWidth="1"/>
-    <col min="5" max="5" width="72.5703125" style="17" customWidth="1"/>
+    <col min="5" max="5" width="72.5703125" style="15" customWidth="1"/>
     <col min="6" max="6" width="24" customWidth="1"/>
   </cols>
   <sheetData>
@@ -739,7 +765,7 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="14" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
@@ -751,72 +777,107 @@
         <v>6</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="15"/>
-      <c r="F2" s="13"/>
-      <c r="H2" s="25"/>
+        <v>15</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="13"/>
+      <c r="F2" s="11"/>
+      <c r="H2" s="19"/>
     </row>
     <row r="3" spans="1:8" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="13"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="19"/>
+    </row>
+    <row r="4" spans="1:8" ht="165.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="21"/>
+      <c r="D4" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="16"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="19"/>
+    </row>
+    <row r="5" spans="1:8" ht="150.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B5" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="13"/>
+      <c r="F5" s="18"/>
+    </row>
+    <row r="6" spans="1:8" ht="195" x14ac:dyDescent="0.25">
+      <c r="A6" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="15"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="25"/>
-    </row>
-    <row r="4" spans="1:8" ht="165.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="21"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="25"/>
-    </row>
-    <row r="5" spans="1:8" ht="150.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="15"/>
-      <c r="F5" s="23"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="25"/>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
+      <c r="B6" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="210" x14ac:dyDescent="0.25">
+      <c r="A7" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="27" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A8" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="27" t="s">
+        <v>34</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -840,15 +901,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>